<commit_message>
Updated the tech stack document.
</commit_message>
<xml_diff>
--- a/TechStackDocumentation.xlsx
+++ b/TechStackDocumentation.xlsx
@@ -47,16 +47,16 @@
     <t>CodingChallenge1</t>
   </si>
   <si>
-    <t>C#, .NET Core, MVC, Web API, REST, ADO.NET, xUnit testing, Moq, Bootstrap, Unobtrusive JavaScript</t>
-  </si>
-  <si>
     <t>C#, .NET Core, MVC, xUnit testing, Moq, Bootstrap, Unobtrusive JavaScript</t>
   </si>
   <si>
     <t>C#, .NET Core, xUnit testing</t>
   </si>
   <si>
-    <t>C#, .NET Core, MVC, Web API, REST, ADO.NET, xUnit testing, Moq, Bootstrap, Unobtrusive JavaScript, SOA</t>
+    <t>C#, .NET Core, MVC, Web API, REST, ADO.NET, xUnit testing, Moq, Bootstrap, Unobtrusive JavaScript, Nlog</t>
+  </si>
+  <si>
+    <t>C#, .NET Core, MVC, Web API, REST, ADO.NET, xUnit testing, Moq, Bootstrap, Unobtrusive JavaScript, Swagger, SOA</t>
   </si>
 </sst>
 </file>
@@ -420,7 +420,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -428,7 +428,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -436,7 +436,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified an existing solution by using microservices architecture where SOLID principles were applied along with unit testing.
</commit_message>
<xml_diff>
--- a/TechStackDocumentation.xlsx
+++ b/TechStackDocumentation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>App Name</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>C#, .NET Core, MVC, Web API, REST, ADO.NET, xUnit testing, Moq, Bootstrap, Unobtrusive JavaScript, Swagger, SOA</t>
+  </si>
+  <si>
+    <t>C#, .NET Core, MVC, Web API, REST, ADO.NET, Nunit testing, Moq, Nlog, Ocelot API Gateway, Exception handeling, Microservices</t>
+  </si>
+  <si>
+    <t>MicroservicesExperiments\Geodesics</t>
   </si>
 </sst>
 </file>
@@ -383,15 +389,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="1" max="1" width="35.109375" customWidth="1"/>
     <col min="2" max="2" width="107.44140625" customWidth="1"/>
     <col min="3" max="3" width="72.109375" customWidth="1"/>
   </cols>
@@ -439,6 +445,14 @@
         <v>8</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>